<commit_message>
ADDING TOP FILE test bench
</commit_message>
<xml_diff>
--- a/Documentation/Test_Cases/Trigger Detection_Test_Cases.xlsx
+++ b/Documentation/Test_Cases/Trigger Detection_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GITHUB\Time_Travelers_Verilog_Stopwatch\Documentation\Test_Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBD0429-F34C-4DD9-A619-03B7EB485555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A4D197-8819-4170-84AB-197013D5CC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -160,6 +160,22 @@
     <t>At first and third observation, 'o_latchcount'=1 and 'o_counterenb'=1
 At second and fourth observation, 'o_latchcount'=0
 'o_counterenb'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>o_latchcount'=0
+'o_counterenb'=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6c32a9f</t>
+  </si>
+  <si>
+    <t>6c32a9f</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -218,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -241,6 +257,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -536,7 +558,7 @@
     <col min="4" max="4" width="37.75" customWidth="1"/>
     <col min="5" max="5" width="16.75" customWidth="1"/>
     <col min="6" max="6" width="42.5" customWidth="1"/>
-    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="7" max="7" width="41.58203125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="13.9140625" customWidth="1"/>
   </cols>
@@ -589,6 +611,15 @@
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -609,6 +640,15 @@
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -629,6 +669,15 @@
       <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -648,6 +697,15 @@
       </c>
       <c r="F5" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>